<commit_message>
Implement camera connection with mobile
</commit_message>
<xml_diff>
--- a/reports/employee_safety.xlsx
+++ b/reports/employee_safety.xlsx
@@ -485,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2026-02-27 20:31:40</t>
+          <t>Generated: 2026-02-28 15:48:19</t>
         </is>
       </c>
     </row>
@@ -562,17 +562,17 @@
     <row r="4" ht="22" customHeight="1">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>EMP-002</t>
+          <t>EMP-001</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Shashidhar Pawadashetti</t>
+          <t>Sambram Sangalad</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>Construction</t>
+          <t>Manufacturing</t>
         </is>
       </c>
       <c r="D4" s="5" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>2026-02-27 23:07:03</t>
+          <t>2026-02-28 15:49:51</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr">
@@ -604,17 +604,17 @@
     <row r="5" ht="22" customHeight="1">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>EMP-003</t>
+          <t>EMP-002</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Sujal Ashok Vaidya</t>
+          <t>Shashidhar Pawadashetti</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>Manufacturing</t>
+          <t>Construction</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>2026-02-27 23:06:38</t>
+          <t>2026-02-28 15:50:18</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr">
@@ -646,40 +646,82 @@
     <row r="6" ht="22" customHeight="1">
       <c r="A6" s="4" t="inlineStr">
         <is>
+          <t>EMP-003</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Sujal Ashok Vaidya</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>Manufacturing</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>✗</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>NOT READY</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-28 15:50:40</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>Missing PPE: Helmet, Safety Vest</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="22" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
           <t>EMP-004</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Vaibhav Hujaratti</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Electrical</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>✗</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
         <is>
           <t>✗</t>
         </is>
       </c>
-      <c r="F6" s="6" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>NOT READY</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>2026-02-27 23:06:52</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>2026-02-28 15:51:54</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>Missing PPE: Helmet, Safety Vest</t>
         </is>

</xml_diff>

<commit_message>
Update model & camera source
</commit_message>
<xml_diff>
--- a/reports/employee_safety.xlsx
+++ b/reports/employee_safety.xlsx
@@ -634,7 +634,7 @@
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>2026-02-28 15:50:18</t>
+          <t>2026-03-01 20:26:11</t>
         </is>
       </c>
       <c r="H5" s="4" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>2026-02-28 15:50:40</t>
+          <t>2026-03-01 20:26:01</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t>2026-02-28 15:51:54</t>
+          <t>2026-03-01 20:25:48</t>
         </is>
       </c>
       <c r="H7" s="4" t="inlineStr">

</xml_diff>